<commit_message>
Update assembly guide to V1.2
- Replaced visual BOM with table.
- Updated component numbers to match build order
- captured and added photos of battery and screws
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/OpenAT_Switch_Latch_BOM.xlsx
+++ b/Documentation/Working_Documents/OpenAT_Switch_Latch_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/Jake/Shared Documents/General/GitHub/OpenAT-Switch-Latch/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{C0EC94A5-2BDB-482C-8925-A43ED8CD790A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAD51FE4-EF9B-481E-8A35-BC47EF4EFCB1}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{C0EC94A5-2BDB-482C-8925-A43ED8CD790A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A13A8FB4-FC28-44E9-9D64-BE34D3EED6E3}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="600" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpenAT Switch Latch BOM V1.0" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>OpenAT Switch Latch</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Commercial Parts</t>
-  </si>
-  <si>
-    <t>Part type (Electrical. Mechanical, Sanitization, etc)</t>
   </si>
   <si>
     <t>Part Name</t>
@@ -884,13 +881,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25228E77-4763-43C3-812A-33F72B26FF01}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.85546875" customWidth="1"/>
@@ -921,10 +918,10 @@
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>75</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="5">
@@ -951,49 +948,49 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="C4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="E4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="H4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="22" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="22">
         <v>1</v>
@@ -1013,18 +1010,18 @@
         <v>0.94</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>21</v>
       </c>
       <c r="D6" s="22">
         <v>2</v>
@@ -1044,18 +1041,18 @@
         <v>4.5</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>24</v>
       </c>
       <c r="D7" s="22">
         <v>2</v>
@@ -1075,18 +1072,18 @@
         <v>5.6</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>27</v>
       </c>
       <c r="D8" s="22">
         <v>1</v>
@@ -1106,18 +1103,18 @@
         <v>0.15</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>30</v>
       </c>
       <c r="D9" s="22">
         <v>1</v>
@@ -1137,18 +1134,18 @@
         <v>0.15</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>33</v>
       </c>
       <c r="D10" s="22">
         <v>1</v>
@@ -1168,18 +1165,18 @@
         <v>0.15</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>36</v>
       </c>
       <c r="D11" s="22">
         <v>1</v>
@@ -1199,18 +1196,18 @@
         <v>0.46</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>39</v>
       </c>
       <c r="D12" s="22">
         <v>1</v>
@@ -1230,18 +1227,18 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="22">
         <v>1</v>
@@ -1261,18 +1258,18 @@
         <v>1.69</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="22">
         <v>1</v>
@@ -1292,18 +1289,18 @@
         <v>0.46</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>46</v>
       </c>
       <c r="D15" s="22">
         <v>1</v>
@@ -1323,15 +1320,15 @@
         <v>0.75</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>49</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="22">
@@ -1352,16 +1349,16 @@
         <v>3.66</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="22">
@@ -1383,10 +1380,10 @@
     </row>
     <row r="18" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>51</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>52</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22">
@@ -1411,48 +1408,48 @@
     </row>
     <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="E21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="F21" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="G21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="H21" s="15" t="s">
         <v>11</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>12</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>55</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>56</v>
       </c>
       <c r="D22" s="22">
         <v>1</v>
@@ -1476,10 +1473,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="22" t="s">
         <v>57</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>58</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="22">
@@ -1511,7 +1508,7 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="26">
         <v>25</v>
@@ -1524,31 +1521,31 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="32" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>61</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="G26" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="15" t="s">
-        <v>64</v>
-      </c>
       <c r="H26" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
@@ -1569,7 +1566,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -1590,7 +1587,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
@@ -1611,7 +1608,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
@@ -1632,7 +1629,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
@@ -1654,7 +1651,7 @@
     <row r="32" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="E32" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="34">
         <f>SUM(F27:F31)</f>
@@ -1665,7 +1662,7 @@
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="25"/>
       <c r="C35" s="10"/>
@@ -1682,18 +1679,18 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1721,12 +1718,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e718a8af-5d48-45b1-a7fb-cef00c107a7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="715913e6-4bf0-458f-8160-f18e142d04ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1945,20 +1944,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e718a8af-5d48-45b1-a7fb-cef00c107a7a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="715913e6-4bf0-458f-8160-f18e142d04ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
+    <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1983,12 +1983,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
-    <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>